<commit_message>
update the report of DGA1031
</commit_message>
<xml_diff>
--- a/DGA1031/Technical Report/Report.xlsx
+++ b/DGA1031/Technical Report/Report.xlsx
@@ -14,8 +14,10 @@
     <sheet name="Reference_9" sheetId="3" r:id="rId5"/>
     <sheet name="Reference_10" sheetId="2" r:id="rId6"/>
     <sheet name="Reference_13" sheetId="6" r:id="rId7"/>
+    <sheet name="PAPER_CONF_J" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Technical Report</t>
   </si>
@@ -1204,6 +1206,9 @@
   </si>
   <si>
     <t>http://dyslexiahelp.umich.edu/tools/apps</t>
+  </si>
+  <si>
+    <t>http://www.scimagojr.com/journalrank.php?category=1706&amp;order=sjr&amp;ord=desc</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1294,6 +1299,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1326,7 +1349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1367,6 +1390,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1376,10 +1421,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1686,10 +1773,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I6" sqref="I6"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,16 +1794,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="4"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1737,19 +1824,19 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1765,16 +1852,16 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1808,55 +1895,55 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="256.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="17" t="s">
+    <row r="7" spans="1:11" s="29" customFormat="1" ht="256.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="11" t="s">
+    <row r="8" spans="1:11" s="34" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="10" t="s">
+      <c r="I8" s="30"/>
+      <c r="J8" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="32" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1887,62 +1974,62 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11" t="s">
+    <row r="10" spans="1:11" s="34" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="210" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="17" t="s">
+    <row r="11" spans="1:11" s="21" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" ht="375" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -1955,35 +2042,35 @@
         <v>76</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="15" t="s">
         <v>78</v>
       </c>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="307.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="17" t="s">
+    <row r="13" spans="1:11" s="40" customFormat="1" ht="307.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="5"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -1999,19 +2086,19 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -2417,4 +2504,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>